<commit_message>
Folder restructuring. Add Development log for Sensor Node.
</commit_message>
<xml_diff>
--- a/Sensor Node/BOM.xlsx
+++ b/Sensor Node/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshar\Documents\capstone\Sensor Node\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CBA019-542B-495F-8FF5-D71D8D686EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C55506-E3A5-40E9-85AB-289F1D5883CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{2B5D9235-DF46-44CC-9AF7-8674BD6918E2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{2B5D9235-DF46-44CC-9AF7-8674BD6918E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sensor Node Board" sheetId="1" r:id="rId1"/>
@@ -572,22 +572,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27170B68-BD39-46D8-8B64-57BBAA09E5C8}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
     <col min="5" max="5" width="35" customWidth="1"/>
-    <col min="6" max="6" width="86.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="150.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="86.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="150.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -610,7 +610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -634,7 +634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -658,7 +658,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -682,7 +682,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -706,7 +706,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -730,7 +730,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -754,7 +754,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -970,20 +970,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1cd51a1f-bf7d-4364-9278-31fd522647f4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1cd51a1f-bf7d-4364-9278-31fd522647f4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1005,14 +1005,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{929EE3F9-2BAC-4C02-9158-3F77C694C7B7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{327D594B-0A95-4722-B9FE-01DFBF087969}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1026,4 +1018,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{929EE3F9-2BAC-4C02-9158-3F77C694C7B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>